<commit_message>
Enhanced For Demo 3
</commit_message>
<xml_diff>
--- a/Data/File _Templates/WorkLog_Template.xlsx
+++ b/Data/File _Templates/WorkLog_Template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112FDAA4-A294-492F-983B-E957205F9083}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C15A3AB-E5C8-4242-B83C-FA8A23CADEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>STATUS</t>
   </si>
@@ -25,6 +25,12 @@
   </si>
   <si>
     <t>ACCOUNT_NAME</t>
+  </si>
+  <si>
+    <t>NUMBER_OF_RECONCILE</t>
+  </si>
+  <si>
+    <t>NUMBER_OF_DISCUSS</t>
   </si>
 </sst>
 </file>
@@ -74,11 +80,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -433,10 +436,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -447,29 +450,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>